<commit_message>
store data in deffrent excel file
</commit_message>
<xml_diff>
--- a/public/images/formData.xlsx
+++ b/public/images/formData.xlsx
@@ -11,36 +11,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>user id</t>
-  </si>
-  <si>
-    <t>user Name</t>
-  </si>
-  <si>
-    <t>user Email</t>
-  </si>
-  <si>
-    <t>user password</t>
-  </si>
-  <si>
-    <t>user imageurl</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+  <si>
+    <t>userid</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>useremail</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>userfaceUrl</t>
+  </si>
+  <si>
+    <t>9zk7nubbtluw8rv5q</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Rutvik</t>
-  </si>
-  <si>
-    <t>rutvik@12gmail.com</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>{"0":-0.16302567720413208,"1":0.2342441827058792,"2":-0.0013093040324747562,"3":-0.10280681401491165,"4":-0.007800218183547258,"5":-0.007871615700423717,"6":-0.04036034643650055,"7":-0.10770491510629654,"8":0.18871471285820007,"9":-0.0280887670814991,"10":0.27825841307640076,"11":0.04250439628958702,"12":-0.21357011795043945,"13":-0.10066569596529007,"14":-0.056301843374967575,"15":0.10320108383893967,"16":-0.2352055162191391,"17":-0.18056771159172058,"18":-0.04761156067252159,"19":-0.1282537430524826,"20":0.0949699804186821,"21":0.06825456023216248,"22":-0.03291900083422661,"23":0.08883036673069,"24":-0.17405566573143005,"25":-0.2566075026988983,"26":-0.03970380872488022,"27":-0.11332967132329941,"28":0.10731203109025955,"29":-0.1168568879365921,"30":0.02322964370250702,"31":-0.023158440366387367,"32":-0.1984214037656784,"33":-0.04563884064555168,"34":0.031411148607730865,"35":0.04098408669233322,"36":0.054543208330869675,"37":-0.06519845128059387,"38":0.2254025936126709,"39":0.02015095390379429,"40":-0.09284184128046036,"41":-0.01373329758644104,"42":0.09145060926675797,"43":0.37168723344802856,"44":0.14217433333396912,"45":-0.01269894652068615,"46":0.021983953192830086,"47":-0.03733644261956215,"48":0.09732963889837265,"49":-0.1894420087337494,"50":0.06964773684740067,"51":0.16549921035766602,"52":0.12568551301956177,"53":0.05270816758275032,"54":0.06410787254571915,"55":-0.19761532545089722,"56":-0.0052104247733950615,"57":0.07557316869497299,"58":-0.2149881273508072,"59":0.08315981179475784,"60":0.060225583612918854,"61":-0.05247300863265991,"62":-0.058412060141563416,"63":-0.0348864421248436,"64":0.21806524693965912,"65":0.08707146346569061,"66":-0.13164861500263214,"67":-0.19154219329357147,"68":0.11916470527648926,"69":-0.12046879529953003,"70":-0.08171297609806061,"71":0.06716793775558472,"72":-0.09970057010650635,"73":-0.11239821463823318,"74":-0.3031514883041382,"75":0.07810866832733154,"76":0.40602394938468933,"77":0.14697134494781494,"78":-0.1692923754453659,"79":0.09608995914459229,"80":-0.08511925488710403,"81":-0.05251413211226463,"82":0.05816803127527237,"83":0.021393919363617897,"84":-0.15832188725471497,"85":0.054387450218200684,"86":-0.13381707668304443,"87":0.08091133087873459,"88":0.18670760095119476,"89":0.09396706521511078,"90":-0.09014914184808731,"91":0.20818978548049927,"92":-0.01232948899269104,"93":-0.021136589348316193,"94":0.051906488835811615,"95":0.08346497267484665,"96":-0.14136701822280884,"97":-0.016982989385724068,"98":-0.08909381926059723,"99":-0.019405260682106018,"100":0.059305232018232346,"101":-0.06516242772340775,"102":0.02418128214776516,"103":0.16825444996356964,"104":-0.18916380405426025,"105":0.08448465168476105,"106":0.018752939999103546,"107":-0.011688909493386745,"108":-0.060829177498817444,"109":0.08777765184640884,"110":-0.13819310069084167,"111":-0.06032150983810425,"112":0.11950813233852386,"113":-0.2554520070552826,"114":0.18363258242607117,"115":0.14241920411586761,"116":0.06580910086631775,"117":0.13090451061725616,"118":0.11518881469964981,"119":0.01425518561154604,"120":0.02173534594476223,"121":0.00171617919113487,"122":-0.09199713915586472,"123":-0.10329621285200119,"124":0.018371393904089928,"125":-0.03783848136663437,"126":0.14093735814094543,"127":0.043305881321430206}</t>
+    <t>{"0":-0.18322962522506714,"1":0.2064070850610733,"2":0.026015130802989006,"3":-0.05736449360847473,"4":-0.022240174934267998,"5":-0.01272329967468977,"6":-0.036502182483673096,"7":-0.08498280495405197,"8":0.16371192038059235,"9":-0.010632830671966076,"10":0.2515646815299988,"11":0.04791298508644104,"12":-0.1866496056318283,"13":-0.07077886909246445,"14":-0.07061983644962311,"15":0.08703090995550156,"16":-0.21615058183670044,"17":-0.16546568274497986,"18":-0.08598027378320694,"19":-0.13444572687149048,"20":0.04641152545809746,"21":0.05617311969399452,"22":-0.03414323553442955,"23":0.035565197467803955,"24":-0.20974335074424744,"25":-0.27684301137924194,"26":-0.02352028526365757,"27":-0.09092475473880768,"28":0.09704017639160156,"29":-0.09487919509410858,"30":0.045347873121500015,"31":-0.03364923223853111,"32":-0.2097923457622528,"33":-0.044465724378824234,"34":0.0443798303604126,"35":0.06176907196640968,"36":-0.001010522129945457,"37":-0.05539001151919365,"38":0.2388012856245041,"39":0.000999712967313826,"40":-0.10115726292133331,"41":0.03114108182489872,"42":0.11585049331188202,"43":0.3301307260990143,"44":0.13646385073661804,"45":0.012258036993443966,"46":0.012249213643372059,"47":-0.06931046396493912,"48":0.0798402950167656,"49":-0.18870915472507477,"50":0.07875624299049377,"51":0.1805676519870758,"52":0.07763119041919708,"53":0.06669747829437256,"54":0.05236174166202545,"55":-0.19541777670383453,"56":0.010519624687731266,"57":0.06189076229929924,"58":-0.22462017834186554,"59":0.05753722041845322,"60":0.044551555067300797,"61":-0.08310028165578842,"62":-0.08822333812713623,"63":-0.0055792140774428844,"64":0.19803865253925323,"65":0.13159707188606262,"66":-0.10665751248598099,"67":-0.201014444231987,"68":0.14996105432510376,"69":-0.14132849872112274,"70":-0.05365066975355148,"71":0.03611328452825546,"72":-0.048990726470947266,"73":-0.10824505984783173,"74":-0.31054240465164185,"75":0.08440668880939484,"76":0.425926148891449,"77":0.12999191880226135,"78":-0.16644300520420074,"79":0.11551357060670853,"80":-0.07487194240093231,"81":-0.06143009290099144,"82":0.06878103315830231,"83":0.053220782428979874,"84":-0.1736316829919815,"85":0.016521165147423744,"86":-0.11116946488618851,"87":0.06857948750257492,"88":0.1636417657136917,"89":0.11347392201423645,"90":-0.0938216969370842,"91":0.1443665325641632,"92":0.026207055896520615,"93":-0.024318447336554527,"94":0.09149383753538132,"95":0.06562624126672745,"96":-0.19301852583885193,"97":-0.03728647530078888,"98":-0.09898153692483902,"99":-0.03784303367137909,"100":0.06756953150033951,"101":-0.039191149175167084,"102":0.03764297813177109,"103":0.16627594828605652,"104":-0.1492624431848526,"105":0.1272362917661667,"106":0.026514194905757904,"107":-0.047301582992076874,"108":-0.02198607847094536,"109":0.09038128703832626,"110":-0.08574368059635162,"111":-0.07558047026395798,"112":0.09492600709199905,"113":-0.24732257425785065,"114":0.21907185018062592,"115":0.11005926132202148,"116":0.03679228201508522,"117":0.17262326180934906,"118":0.15408888459205627,"119":0.037930313497781754,"120":0.015967775136232376,"121":0.07823996245861053,"122":-0.10149620473384857,"123":-0.10199502855539322,"124":-0.03092358447611332,"125":-0.03962467238306999,"126":0.16025269031524658,"127":0.05673786625266075}</t>
   </si>
 </sst>
 </file>
@@ -445,13 +439,13 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
store to excel sheet
</commit_message>
<xml_diff>
--- a/public/images/formData.xlsx
+++ b/public/images/formData.xlsx
@@ -28,13 +28,13 @@
     <t>userfaceUrl</t>
   </si>
   <si>
-    <t>9zk7nubbtluw8rv5q</t>
+    <t>ue2qbx9q8luxoccm2</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>{"0":-0.18322962522506714,"1":0.2064070850610733,"2":0.026015130802989006,"3":-0.05736449360847473,"4":-0.022240174934267998,"5":-0.01272329967468977,"6":-0.036502182483673096,"7":-0.08498280495405197,"8":0.16371192038059235,"9":-0.010632830671966076,"10":0.2515646815299988,"11":0.04791298508644104,"12":-0.1866496056318283,"13":-0.07077886909246445,"14":-0.07061983644962311,"15":0.08703090995550156,"16":-0.21615058183670044,"17":-0.16546568274497986,"18":-0.08598027378320694,"19":-0.13444572687149048,"20":0.04641152545809746,"21":0.05617311969399452,"22":-0.03414323553442955,"23":0.035565197467803955,"24":-0.20974335074424744,"25":-0.27684301137924194,"26":-0.02352028526365757,"27":-0.09092475473880768,"28":0.09704017639160156,"29":-0.09487919509410858,"30":0.045347873121500015,"31":-0.03364923223853111,"32":-0.2097923457622528,"33":-0.044465724378824234,"34":0.0443798303604126,"35":0.06176907196640968,"36":-0.001010522129945457,"37":-0.05539001151919365,"38":0.2388012856245041,"39":0.000999712967313826,"40":-0.10115726292133331,"41":0.03114108182489872,"42":0.11585049331188202,"43":0.3301307260990143,"44":0.13646385073661804,"45":0.012258036993443966,"46":0.012249213643372059,"47":-0.06931046396493912,"48":0.0798402950167656,"49":-0.18870915472507477,"50":0.07875624299049377,"51":0.1805676519870758,"52":0.07763119041919708,"53":0.06669747829437256,"54":0.05236174166202545,"55":-0.19541777670383453,"56":0.010519624687731266,"57":0.06189076229929924,"58":-0.22462017834186554,"59":0.05753722041845322,"60":0.044551555067300797,"61":-0.08310028165578842,"62":-0.08822333812713623,"63":-0.0055792140774428844,"64":0.19803865253925323,"65":0.13159707188606262,"66":-0.10665751248598099,"67":-0.201014444231987,"68":0.14996105432510376,"69":-0.14132849872112274,"70":-0.05365066975355148,"71":0.03611328452825546,"72":-0.048990726470947266,"73":-0.10824505984783173,"74":-0.31054240465164185,"75":0.08440668880939484,"76":0.425926148891449,"77":0.12999191880226135,"78":-0.16644300520420074,"79":0.11551357060670853,"80":-0.07487194240093231,"81":-0.06143009290099144,"82":0.06878103315830231,"83":0.053220782428979874,"84":-0.1736316829919815,"85":0.016521165147423744,"86":-0.11116946488618851,"87":0.06857948750257492,"88":0.1636417657136917,"89":0.11347392201423645,"90":-0.0938216969370842,"91":0.1443665325641632,"92":0.026207055896520615,"93":-0.024318447336554527,"94":0.09149383753538132,"95":0.06562624126672745,"96":-0.19301852583885193,"97":-0.03728647530078888,"98":-0.09898153692483902,"99":-0.03784303367137909,"100":0.06756953150033951,"101":-0.039191149175167084,"102":0.03764297813177109,"103":0.16627594828605652,"104":-0.1492624431848526,"105":0.1272362917661667,"106":0.026514194905757904,"107":-0.047301582992076874,"108":-0.02198607847094536,"109":0.09038128703832626,"110":-0.08574368059635162,"111":-0.07558047026395798,"112":0.09492600709199905,"113":-0.24732257425785065,"114":0.21907185018062592,"115":0.11005926132202148,"116":0.03679228201508522,"117":0.17262326180934906,"118":0.15408888459205627,"119":0.037930313497781754,"120":0.015967775136232376,"121":0.07823996245861053,"122":-0.10149620473384857,"123":-0.10199502855539322,"124":-0.03092358447611332,"125":-0.03962467238306999,"126":0.16025269031524658,"127":0.05673786625266075}</t>
+    <t>{"0":-0.162633016705513,"1":0.1973511129617691,"2":0.05015500634908676,"3":-0.03953949362039566,"4":-0.03331030160188675,"5":0.009493923746049404,"6":-0.028154879808425903,"7":-0.06832894682884216,"8":0.15125001966953278,"9":0.020595187321305275,"10":0.24499602615833282,"11":0.06400331109762192,"12":-0.22593925893306732,"13":-0.0395185686647892,"14":-0.10580717027187347,"15":0.10613147169351578,"16":-0.19612787663936615,"17":-0.14663730561733246,"18":-0.12322859466075897,"19":-0.12788182497024536,"20":0.06113014370203018,"21":0.08724340051412582,"22":-0.027959084138274193,"23":0.015539347194135189,"24":-0.22177359461784363,"25":-0.26985934376716614,"26":-0.01496500801295042,"27":-0.07361457496881485,"28":0.0717867910861969,"29":-0.13154126703739166,"30":0.05786324664950371,"31":-0.015289557166397572,"32":-0.22231915593147278,"33":-0.059564169496297836,"34":0.027443747967481613,"35":0.06295355409383774,"36":0.004954797215759754,"37":-0.08295457810163498,"38":0.21505680680274963,"39":0.04940776526927948,"40":-0.11201681196689606,"41":0.05439417064189911,"42":0.10504181683063507,"43":0.3644810914993286,"44":0.1808539777994156,"45":0.01854855567216873,"46":0.01841064915060997,"47":-0.07657255977392197,"48":0.11365706473588943,"49":-0.240988627076149,"50":0.10342460125684738,"51":0.13160039484500885,"52":0.11047572642564774,"53":0.0766943022608757,"54":0.08778838068246841,"55":-0.2130214124917984,"56":0.03144310042262077,"57":0.10751143097877502,"58":-0.2010337859392166,"59":0.04611331596970558,"60":0.03219122812151909,"61":-0.02818486839532852,"62":-0.033547915518283844,"63":-0.01122575905174017,"64":0.17258211970329285,"65":0.07836860418319702,"66":-0.09610659629106522,"67":-0.15032042562961578,"68":0.12963330745697021,"69":-0.10297084599733353,"70":-0.057694822549819946,"71":0.05186950042843819,"72":-0.06956522166728973,"73":-0.12262360006570816,"74":-0.36059340834617615,"75":0.1189107820391655,"76":0.470702588558197,"77":0.1282406449317932,"78":-0.19410216808319092,"79":0.0833299532532692,"80":-0.044275227934122086,"81":-0.026552598923444748,"82":0.10044535249471664,"83":0.027390845119953156,"84":-0.16930551826953888,"85":-0.022380374372005463,"86":-0.12111600488424301,"87":0.059997592121362686,"88":0.19354528188705444,"89":0.10884181410074234,"90":-0.12576830387115479,"91":0.15404367446899414,"92":0.033426977694034576,"93":-0.046532195061445236,"94":0.08753460645675659,"95":0.07801196724176407,"96":-0.17903776466846466,"97":-0.00019945604435633868,"98":-0.1083666980266571,"99":-0.025601718574762344,"100":0.06873480975627899,"101":-0.026713749393820763,"102":0.010991417802870274,"103":0.16991102695465088,"104":-0.1651907116174698,"105":0.12200672179460526,"106":0.03307827189564705,"107":-0.04508204013109207,"108":-0.015049159526824951,"109":0.05297211557626724,"110":-0.12770946323871613,"111":-0.0337783582508564,"112":0.11236095428466797,"113":-0.27835580706596375,"114":0.20537357032299042,"115":0.1374458223581314,"116":0.006035256199538708,"117":0.15464916825294495,"118":0.14985838532447815,"119":0.024170830845832825,"120":0.01860850676894188,"121":0.0933075100183487,"122":-0.11189769953489304,"123":-0.10500682890415192,"124":0.036279190331697464,"125":-0.04607169330120087,"126":0.14097340404987335,"127":0.05128635838627815}</t>
   </si>
 </sst>
 </file>

</xml_diff>